<commit_message>
ya casi pero ya casoiiii
</commit_message>
<xml_diff>
--- a/estudiantes_sustentacion_proyecto.xlsx
+++ b/estudiantes_sustentacion_proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Music\PryHorarioTesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58911175-5091-4697-8368-503580447F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BA0774-01D9-4778-AFD6-67457DB6D271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72140228-D5D8-4C8D-AF3F-2AD74FCA34C0}"/>
   </bookViews>
@@ -1131,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43142032-E38A-45CE-837D-9E934073690F}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="B50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>